<commit_message>
!them truong statusID tren bang Complaint & Request Ngoc.phan
</commit_message>
<xml_diff>
--- a/Document/table.xlsx
+++ b/Document/table.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="75" windowWidth="19095" windowHeight="11760"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
   <si>
     <t>USER</t>
   </si>
@@ -147,8 +147,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -199,6 +199,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -277,6 +282,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -311,6 +317,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -486,16 +493,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D9:O29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="9.140625" style="1"/>
+    <col min="1" max="3" width="9.140625" style="1"/>
+    <col min="4" max="4" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9.140625" style="1"/>
     <col min="7" max="7" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.140625" style="1"/>
     <col min="9" max="9" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
@@ -505,7 +514,7 @@
     <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="9" spans="4:15">
+    <row r="9" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D9" s="2" t="s">
         <v>0</v>
       </c>
@@ -525,7 +534,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="4:15">
+    <row r="10" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D10" s="1" t="s">
         <v>1</v>
       </c>
@@ -545,7 +554,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="4:15">
+    <row r="11" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D11" s="1" t="s">
         <v>2</v>
       </c>
@@ -565,7 +574,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="4:15">
+    <row r="12" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D12" s="1" t="s">
         <v>3</v>
       </c>
@@ -576,7 +585,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="4:15">
+    <row r="13" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D13" s="1" t="s">
         <v>5</v>
       </c>
@@ -587,15 +596,18 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="4:15">
+    <row r="14" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D14" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="I14" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="M14" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="4:15">
+    <row r="15" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D15" s="1" t="s">
         <v>7</v>
       </c>
@@ -603,12 +615,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="4:15">
+    <row r="16" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D16" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="4:12">
+      <c r="M16" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D23" s="2" t="s">
         <v>27</v>
       </c>
@@ -622,7 +637,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="4:12">
+    <row r="24" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D24" s="1" t="s">
         <v>28</v>
       </c>
@@ -636,7 +651,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="4:12">
+    <row r="25" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D25" s="1" t="s">
         <v>31</v>
       </c>
@@ -650,7 +665,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="4:12">
+    <row r="26" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D26" s="1" t="s">
         <v>20</v>
       </c>
@@ -661,7 +676,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="4:12">
+    <row r="27" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D27" s="1" t="s">
         <v>32</v>
       </c>
@@ -672,12 +687,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="4:12">
+    <row r="28" spans="4:12" x14ac:dyDescent="0.25">
       <c r="G28" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="4:12">
+    <row r="29" spans="4:12" x14ac:dyDescent="0.25">
       <c r="G29" s="1" t="s">
         <v>41</v>
       </c>
@@ -688,24 +703,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Chia công việc "use case specification", trong sheet Task
</commit_message>
<xml_diff>
--- a/Document/table.xlsx
+++ b/Document/table.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="75" windowWidth="19095" windowHeight="11760"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Database" sheetId="1" r:id="rId1"/>
+    <sheet name="Task" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <fileRecoveryPr autoRecover="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="63">
   <si>
     <t>USER</t>
   </si>
@@ -142,13 +143,76 @@
   </si>
   <si>
     <t>labStatus(boolean)</t>
+  </si>
+  <si>
+    <t>Ngọc</t>
+  </si>
+  <si>
+    <t>Sơn</t>
+  </si>
+  <si>
+    <t>Vân</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>1. Addressing complaint</t>
+  </si>
+  <si>
+    <t>2. Config management</t>
+  </si>
+  <si>
+    <t>3. Maintain document</t>
+  </si>
+  <si>
+    <t>5. Log out</t>
+  </si>
+  <si>
+    <t>4. Log in</t>
+  </si>
+  <si>
+    <t>6. Create complain</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>7. Keep track of the lab</t>
+  </si>
+  <si>
+    <t>8. Create user</t>
+  </si>
+  <si>
+    <t>9. Assign request</t>
+  </si>
+  <si>
+    <t>10. Check report</t>
+  </si>
+  <si>
+    <t>11. Assign complain</t>
+  </si>
+  <si>
+    <t>12. Response request</t>
+  </si>
+  <si>
+    <t>13. Create request</t>
+  </si>
+  <si>
+    <t>14. View status complain</t>
+  </si>
+  <si>
+    <t>15. Update status</t>
+  </si>
+  <si>
+    <t>16. Manage profile</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,8 +220,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -176,8 +248,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -185,14 +281,46 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -282,7 +410,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -317,7 +444,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -493,14 +619,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="D9:O29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="3" width="9.140625" style="1"/>
     <col min="4" max="4" width="14.140625" style="1" bestFit="1" customWidth="1"/>
@@ -514,7 +640,7 @@
     <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="9" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="4:15">
       <c r="D9" s="2" t="s">
         <v>0</v>
       </c>
@@ -534,7 +660,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="4:15">
       <c r="D10" s="1" t="s">
         <v>1</v>
       </c>
@@ -554,7 +680,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="4:15">
       <c r="D11" s="1" t="s">
         <v>2</v>
       </c>
@@ -574,7 +700,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="4:15">
       <c r="D12" s="1" t="s">
         <v>3</v>
       </c>
@@ -585,7 +711,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="4:15">
       <c r="D13" s="1" t="s">
         <v>5</v>
       </c>
@@ -596,7 +722,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="4:15">
       <c r="D14" s="1" t="s">
         <v>6</v>
       </c>
@@ -607,7 +733,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="4:15">
       <c r="D15" s="1" t="s">
         <v>7</v>
       </c>
@@ -615,7 +741,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="4:15">
       <c r="D16" s="1" t="s">
         <v>4</v>
       </c>
@@ -623,7 +749,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:12">
       <c r="D23" s="2" t="s">
         <v>27</v>
       </c>
@@ -637,7 +763,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:12">
       <c r="D24" s="1" t="s">
         <v>28</v>
       </c>
@@ -651,7 +777,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:12">
       <c r="D25" s="1" t="s">
         <v>31</v>
       </c>
@@ -665,7 +791,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:12">
       <c r="D26" s="1" t="s">
         <v>20</v>
       </c>
@@ -676,7 +802,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:12">
       <c r="D27" s="1" t="s">
         <v>32</v>
       </c>
@@ -687,12 +813,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:12">
       <c r="G28" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:12">
       <c r="G29" s="1" t="s">
         <v>41</v>
       </c>
@@ -703,24 +829,210 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B3:E19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="35.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:5" ht="18.75">
+      <c r="B3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5">
+      <c r="B4" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="2:5">
+      <c r="B5" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6" spans="2:5">
+      <c r="B6" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="2:5">
+      <c r="B7" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="2:5">
+      <c r="B8" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="2:5">
+      <c r="B9" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="2:5">
+      <c r="B10" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="2:5">
+      <c r="B11" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="2:5">
+      <c r="B12" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="2:5">
+      <c r="B13" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="2:5">
+      <c r="B14" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" spans="2:5">
+      <c r="B15" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5">
+      <c r="B16" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5">
+      <c r="B17" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5">
+      <c r="B18" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5">
+      <c r="B19" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>